<commit_message>
add backup and update (the before was actualizacion) & call
</commit_message>
<xml_diff>
--- a/excel/excel_nuevos_precios.xlsx
+++ b/excel/excel_nuevos_precios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\Lenguajes\Python\AcutualizacionPreciosCsv\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8D72C6-2A77-4142-B03A-37252FCB4D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77851AC-E063-4393-9EE9-1C51F9AC4519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15EE2AE1-9EDA-498F-ABB8-F5E8E1973CE5}"/>
+    <workbookView xWindow="5790" yWindow="3405" windowWidth="21600" windowHeight="11385" xr2:uid="{15EE2AE1-9EDA-498F-ABB8-F5E8E1973CE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>lavadora</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Producto</t>
+  </si>
+  <si>
+    <t>bomba de agua</t>
   </si>
 </sst>
 </file>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A181350-E048-40E0-95F6-BD27C7F898CD}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,6 +509,24 @@
         <v>500</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>400</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>